<commit_message>
Update Classroom Test score Analysis.xlsx
</commit_message>
<xml_diff>
--- a/Classroom Test score Analysis.xlsx
+++ b/Classroom Test score Analysis.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Students Performance\Students_Performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD969B23-55F5-4984-B94B-747485E8CE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1550A9ED-98CA-440E-9A5B-075096D1E6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="zg3HsRFPrEjDL1F5TjWYCaslAJeCkBfqHS6JhqeyE0cBIP6VRWIbSAtYTjxYy858RKo2zoa/xGWx+6+XRqdydw==" workbookSaltValue="8YgVU5nFUnzzYOJICyTWEA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7918FD85-49B2-40B5-8510-7659F2B014DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="7" activeTab="7" xr2:uid="{7918FD85-49B2-40B5-8510-7659F2B014DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="pivot" sheetId="8" r:id="rId1"/>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
-    <sheet name="Ethnicity" sheetId="3" r:id="rId3"/>
-    <sheet name="Parent's education level" sheetId="4" r:id="rId4"/>
-    <sheet name="Gender" sheetId="5" r:id="rId5"/>
-    <sheet name="lunch type" sheetId="6" r:id="rId6"/>
-    <sheet name="Test preparation course" sheetId="7" r:id="rId7"/>
+    <sheet name="pivot" sheetId="8" state="hidden" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" state="hidden" r:id="rId2"/>
+    <sheet name="Ethnicity" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Parent's education level" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Gender" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="lunch type" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="Test preparation course" sheetId="7" state="hidden" r:id="rId7"/>
     <sheet name="Dashboard" sheetId="2" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Data!$G$2:$G$1001</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Data!$F$2:$F$1001</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Data!$H$2:$H$1001</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Data!$F$2:$F$1001</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Data!$H$2:$H$1001</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Data!$G$2:$G$1001</definedName>
     <definedName name="Slicer_gender">#N/A</definedName>
     <definedName name="Slicer_lunch">#N/A</definedName>
     <definedName name="Slicer_parental_level_of_education">#N/A</definedName>
@@ -34,7 +35,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -985,15 +986,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1040,69 +1041,9 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1131,7 +1072,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1194,7 +1135,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1257,7 +1198,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -14072,7 +14013,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2414A199-2131-4D1C-B5FF-D13ED38C4F7A}" name="Scores_pivot" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2414A199-2131-4D1C-B5FF-D13ED38C4F7A}" name="Scores_pivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D38" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" showAll="0">
@@ -14243,7 +14184,7 @@
     <dataField name="Average writing score" fld="7" subtotal="average" baseField="1" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="16">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -14328,9 +14269,9 @@
     <tableColumn id="3" xr3:uid="{3A690BDC-1B06-4BD8-8792-EC43C54F6830}" name="parental level of education"/>
     <tableColumn id="4" xr3:uid="{0FCCA679-DEFE-43BF-8D81-23414317842D}" name="lunch"/>
     <tableColumn id="5" xr3:uid="{B85EC6EC-5AD8-453E-96BA-53B1582F6751}" name="test preparation course"/>
-    <tableColumn id="6" xr3:uid="{BC04CCFB-2375-4050-B518-2D88D4051896}" name="math score" totalsRowDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{CA23C635-0D99-4A34-BAFF-9A2E43BDD4E4}" name="reading score" totalsRowDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{8B387FE5-2817-4DCC-9E57-EBF84F1EAC5F}" name="writing score" totalsRowDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{BC04CCFB-2375-4050-B518-2D88D4051896}" name="math score" totalsRowDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{CA23C635-0D99-4A34-BAFF-9A2E43BDD4E4}" name="reading score" totalsRowDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{8B387FE5-2817-4DCC-9E57-EBF84F1EAC5F}" name="writing score" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14655,8 +14596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4995FB-CB0D-4D06-89EA-3232D8222092}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" activeCellId="1" sqref="E33 G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14683,7 +14624,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -14702,7 +14643,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="38" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1">
@@ -14716,7 +14657,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1">
@@ -14730,7 +14671,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
@@ -14744,7 +14685,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="1">
@@ -14758,7 +14699,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1">
@@ -14772,7 +14713,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1">
@@ -14786,7 +14727,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="1">
@@ -14800,7 +14741,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="38" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="1">
@@ -14814,7 +14755,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1">
@@ -14828,7 +14769,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1">
@@ -14842,7 +14783,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1">
@@ -14856,7 +14797,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1">
@@ -14870,7 +14811,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1">
@@ -14884,7 +14825,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1">
@@ -14898,7 +14839,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="1">
@@ -14912,7 +14853,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="1">
@@ -14926,7 +14867,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="1">
@@ -14940,7 +14881,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="1">
@@ -14954,7 +14895,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="1">
@@ -14968,7 +14909,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="1">
@@ -14982,7 +14923,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="1">
@@ -14996,7 +14937,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="38" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="1">
@@ -15010,7 +14951,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="1">
@@ -15024,7 +14965,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="1">
@@ -15038,7 +14979,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="1">
@@ -15052,7 +14993,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="1">
@@ -15066,7 +15007,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="1">
@@ -15080,7 +15021,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="1">
@@ -15094,7 +15035,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="38" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="1">
@@ -15108,7 +15049,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B33" s="1">
@@ -15122,7 +15063,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="1">
@@ -15136,7 +15077,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="1">
@@ -15150,7 +15091,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B36" s="1">
@@ -15164,7 +15105,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B37" s="1">
@@ -15178,7 +15119,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="1">
@@ -15201,7 +15142,7 @@
   <dimension ref="A1:Q1006"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41293,7 +41234,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41414,7 +41355,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41552,7 +41493,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41622,7 +41563,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41761,7 +41702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13590E80-9748-4786-84C1-4C034E4B41EA}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
@@ -41776,26 +41717,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E2"/>

</xml_diff>